<commit_message>
TC updated based on Storm-Blackwidow sprint
</commit_message>
<xml_diff>
--- a/TCS_NEWUI_AgGrid.xlsx
+++ b/TCS_NEWUI_AgGrid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sumit Rana\Projects\AdIntel- New\Test Cases\TC Repository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sumit Rana\Projects\AdIntel- New\Test Cases\TC_Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2949F298-A8D7-4EEA-8E1B-B2C894F1C7E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD77FC2-EDA9-43AE-9C59-347BD0C0B08D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2721,6 +2721,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="40" fillId="26" borderId="41" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="26" borderId="42" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="26" borderId="43" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="32" borderId="41" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2738,15 +2747,6 @@
     </xf>
     <xf numFmtId="0" fontId="39" fillId="33" borderId="43" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="26" borderId="41" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="26" borderId="42" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="26" borderId="43" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="26" borderId="22" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4707,8 +4707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15"/>
@@ -5948,12 +5948,12 @@
       <c r="A18" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="B18" s="88" t="s">
+      <c r="B18" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="89"/>
-      <c r="D18" s="89"/>
-      <c r="E18" s="90"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="93"/>
       <c r="F18" s="53" t="s">
         <v>87</v>
       </c>
@@ -5966,14 +5966,14 @@
       <c r="A19" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="91" t="s">
+      <c r="B19" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="92"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="92"/>
-      <c r="F19" s="92"/>
-      <c r="G19" s="93"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="95"/>
+      <c r="F19" s="95"/>
+      <c r="G19" s="96"/>
     </row>
     <row r="20" spans="1:7" s="51" customFormat="1">
       <c r="A20" s="56" t="s">
@@ -6021,23 +6021,23 @@
       <c r="A22" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="94"/>
-      <c r="C22" s="95"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="95"/>
-      <c r="F22" s="95"/>
-      <c r="G22" s="96"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="89"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="89"/>
+      <c r="G22" s="90"/>
     </row>
     <row r="23" spans="1:7" s="51" customFormat="1">
       <c r="A23" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="B23" s="88" t="s">
+      <c r="B23" s="91" t="s">
         <v>105</v>
       </c>
-      <c r="C23" s="89"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="90"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="92"/>
+      <c r="E23" s="93"/>
       <c r="F23" s="53" t="s">
         <v>87</v>
       </c>
@@ -6050,14 +6050,14 @@
       <c r="A24" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="91" t="s">
+      <c r="B24" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="92"/>
-      <c r="D24" s="92"/>
-      <c r="E24" s="92"/>
-      <c r="F24" s="92"/>
-      <c r="G24" s="93"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="95"/>
+      <c r="G24" s="96"/>
     </row>
     <row r="25" spans="1:7" s="51" customFormat="1">
       <c r="A25" s="56" t="s">
@@ -6156,23 +6156,23 @@
       <c r="A30" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B30" s="94"/>
-      <c r="C30" s="95"/>
-      <c r="D30" s="95"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="95"/>
-      <c r="G30" s="96"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="90"/>
     </row>
     <row r="31" spans="1:7" s="51" customFormat="1">
       <c r="A31" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="B31" s="88" t="s">
+      <c r="B31" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="C31" s="89"/>
-      <c r="D31" s="89"/>
-      <c r="E31" s="90"/>
+      <c r="C31" s="92"/>
+      <c r="D31" s="92"/>
+      <c r="E31" s="93"/>
       <c r="F31" s="53" t="s">
         <v>87</v>
       </c>
@@ -6185,14 +6185,14 @@
       <c r="A32" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="91" t="s">
+      <c r="B32" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="92"/>
-      <c r="D32" s="92"/>
-      <c r="E32" s="92"/>
-      <c r="F32" s="92"/>
-      <c r="G32" s="93"/>
+      <c r="C32" s="95"/>
+      <c r="D32" s="95"/>
+      <c r="E32" s="95"/>
+      <c r="F32" s="95"/>
+      <c r="G32" s="96"/>
     </row>
     <row r="33" spans="1:7" s="51" customFormat="1">
       <c r="A33" s="56" t="s">
@@ -6342,23 +6342,23 @@
       <c r="A41" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B41" s="94"/>
-      <c r="C41" s="95"/>
-      <c r="D41" s="95"/>
-      <c r="E41" s="95"/>
-      <c r="F41" s="95"/>
-      <c r="G41" s="96"/>
+      <c r="B41" s="88"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="89"/>
+      <c r="G41" s="90"/>
     </row>
     <row r="42" spans="1:7" s="51" customFormat="1">
       <c r="A42" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="B42" s="88" t="s">
+      <c r="B42" s="91" t="s">
         <v>212</v>
       </c>
-      <c r="C42" s="89"/>
-      <c r="D42" s="89"/>
-      <c r="E42" s="90"/>
+      <c r="C42" s="92"/>
+      <c r="D42" s="92"/>
+      <c r="E42" s="93"/>
       <c r="F42" s="53" t="s">
         <v>87</v>
       </c>
@@ -6371,14 +6371,14 @@
       <c r="A43" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="91" t="s">
+      <c r="B43" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="92"/>
-      <c r="D43" s="92"/>
-      <c r="E43" s="92"/>
-      <c r="F43" s="92"/>
-      <c r="G43" s="93"/>
+      <c r="C43" s="95"/>
+      <c r="D43" s="95"/>
+      <c r="E43" s="95"/>
+      <c r="F43" s="95"/>
+      <c r="G43" s="96"/>
     </row>
     <row r="44" spans="1:7" s="51" customFormat="1">
       <c r="A44" s="56" t="s">
@@ -6458,23 +6458,23 @@
       <c r="A48" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="94"/>
-      <c r="C48" s="95"/>
-      <c r="D48" s="95"/>
-      <c r="E48" s="95"/>
-      <c r="F48" s="95"/>
-      <c r="G48" s="96"/>
+      <c r="B48" s="88"/>
+      <c r="C48" s="89"/>
+      <c r="D48" s="89"/>
+      <c r="E48" s="89"/>
+      <c r="F48" s="89"/>
+      <c r="G48" s="90"/>
     </row>
     <row r="49" spans="1:7" s="51" customFormat="1">
       <c r="A49" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="B49" s="88" t="s">
+      <c r="B49" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="C49" s="89"/>
-      <c r="D49" s="89"/>
-      <c r="E49" s="90"/>
+      <c r="C49" s="92"/>
+      <c r="D49" s="92"/>
+      <c r="E49" s="93"/>
       <c r="F49" s="53" t="s">
         <v>87</v>
       </c>
@@ -6487,14 +6487,14 @@
       <c r="A50" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="91" t="s">
+      <c r="B50" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C50" s="92"/>
-      <c r="D50" s="92"/>
-      <c r="E50" s="92"/>
-      <c r="F50" s="92"/>
-      <c r="G50" s="93"/>
+      <c r="C50" s="95"/>
+      <c r="D50" s="95"/>
+      <c r="E50" s="95"/>
+      <c r="F50" s="95"/>
+      <c r="G50" s="96"/>
     </row>
     <row r="51" spans="1:7" s="51" customFormat="1">
       <c r="A51" s="56" t="s">
@@ -6591,23 +6591,23 @@
       <c r="A56" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B56" s="94"/>
-      <c r="C56" s="95"/>
-      <c r="D56" s="95"/>
-      <c r="E56" s="95"/>
-      <c r="F56" s="95"/>
-      <c r="G56" s="96"/>
+      <c r="B56" s="88"/>
+      <c r="C56" s="89"/>
+      <c r="D56" s="89"/>
+      <c r="E56" s="89"/>
+      <c r="F56" s="89"/>
+      <c r="G56" s="90"/>
     </row>
     <row r="57" spans="1:7" s="51" customFormat="1">
       <c r="A57" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="B57" s="88" t="s">
+      <c r="B57" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="C57" s="89"/>
-      <c r="D57" s="89"/>
-      <c r="E57" s="90"/>
+      <c r="C57" s="92"/>
+      <c r="D57" s="92"/>
+      <c r="E57" s="93"/>
       <c r="F57" s="53" t="s">
         <v>87</v>
       </c>
@@ -6620,14 +6620,14 @@
       <c r="A58" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="91" t="s">
+      <c r="B58" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C58" s="92"/>
-      <c r="D58" s="92"/>
-      <c r="E58" s="92"/>
-      <c r="F58" s="92"/>
-      <c r="G58" s="93"/>
+      <c r="C58" s="95"/>
+      <c r="D58" s="95"/>
+      <c r="E58" s="95"/>
+      <c r="F58" s="95"/>
+      <c r="G58" s="96"/>
     </row>
     <row r="59" spans="1:7" s="51" customFormat="1">
       <c r="A59" s="56" t="s">
@@ -6724,23 +6724,23 @@
       <c r="A64" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B64" s="94"/>
-      <c r="C64" s="95"/>
-      <c r="D64" s="95"/>
-      <c r="E64" s="95"/>
-      <c r="F64" s="95"/>
-      <c r="G64" s="96"/>
+      <c r="B64" s="88"/>
+      <c r="C64" s="89"/>
+      <c r="D64" s="89"/>
+      <c r="E64" s="89"/>
+      <c r="F64" s="89"/>
+      <c r="G64" s="90"/>
     </row>
     <row r="65" spans="1:7" s="51" customFormat="1">
       <c r="A65" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="B65" s="88" t="s">
+      <c r="B65" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="C65" s="89"/>
-      <c r="D65" s="89"/>
-      <c r="E65" s="90"/>
+      <c r="C65" s="92"/>
+      <c r="D65" s="92"/>
+      <c r="E65" s="93"/>
       <c r="F65" s="53" t="s">
         <v>87</v>
       </c>
@@ -6753,14 +6753,14 @@
       <c r="A66" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B66" s="91" t="s">
+      <c r="B66" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C66" s="92"/>
-      <c r="D66" s="92"/>
-      <c r="E66" s="92"/>
-      <c r="F66" s="92"/>
-      <c r="G66" s="93"/>
+      <c r="C66" s="95"/>
+      <c r="D66" s="95"/>
+      <c r="E66" s="95"/>
+      <c r="F66" s="95"/>
+      <c r="G66" s="96"/>
     </row>
     <row r="67" spans="1:7" s="51" customFormat="1">
       <c r="A67" s="56" t="s">
@@ -6840,23 +6840,23 @@
       <c r="A71" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B71" s="94"/>
-      <c r="C71" s="95"/>
-      <c r="D71" s="95"/>
-      <c r="E71" s="95"/>
-      <c r="F71" s="95"/>
-      <c r="G71" s="96"/>
+      <c r="B71" s="88"/>
+      <c r="C71" s="89"/>
+      <c r="D71" s="89"/>
+      <c r="E71" s="89"/>
+      <c r="F71" s="89"/>
+      <c r="G71" s="90"/>
     </row>
     <row r="72" spans="1:7" s="51" customFormat="1">
       <c r="A72" s="52" t="s">
         <v>126</v>
       </c>
-      <c r="B72" s="88" t="s">
+      <c r="B72" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="C72" s="89"/>
-      <c r="D72" s="89"/>
-      <c r="E72" s="90"/>
+      <c r="C72" s="92"/>
+      <c r="D72" s="92"/>
+      <c r="E72" s="93"/>
       <c r="F72" s="53" t="s">
         <v>87</v>
       </c>
@@ -6869,14 +6869,14 @@
       <c r="A73" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B73" s="91" t="s">
+      <c r="B73" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C73" s="92"/>
-      <c r="D73" s="92"/>
-      <c r="E73" s="92"/>
-      <c r="F73" s="92"/>
-      <c r="G73" s="93"/>
+      <c r="C73" s="95"/>
+      <c r="D73" s="95"/>
+      <c r="E73" s="95"/>
+      <c r="F73" s="95"/>
+      <c r="G73" s="96"/>
     </row>
     <row r="74" spans="1:7" s="51" customFormat="1">
       <c r="A74" s="56" t="s">
@@ -6956,23 +6956,23 @@
       <c r="A78" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B78" s="94"/>
-      <c r="C78" s="95"/>
-      <c r="D78" s="95"/>
-      <c r="E78" s="95"/>
-      <c r="F78" s="95"/>
-      <c r="G78" s="96"/>
+      <c r="B78" s="88"/>
+      <c r="C78" s="89"/>
+      <c r="D78" s="89"/>
+      <c r="E78" s="89"/>
+      <c r="F78" s="89"/>
+      <c r="G78" s="90"/>
     </row>
     <row r="79" spans="1:7" s="51" customFormat="1">
       <c r="A79" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="B79" s="88" t="s">
+      <c r="B79" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="C79" s="89"/>
-      <c r="D79" s="89"/>
-      <c r="E79" s="90"/>
+      <c r="C79" s="92"/>
+      <c r="D79" s="92"/>
+      <c r="E79" s="93"/>
       <c r="F79" s="53" t="s">
         <v>87</v>
       </c>
@@ -6985,14 +6985,14 @@
       <c r="A80" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B80" s="91" t="s">
+      <c r="B80" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C80" s="92"/>
-      <c r="D80" s="92"/>
-      <c r="E80" s="92"/>
-      <c r="F80" s="92"/>
-      <c r="G80" s="93"/>
+      <c r="C80" s="95"/>
+      <c r="D80" s="95"/>
+      <c r="E80" s="95"/>
+      <c r="F80" s="95"/>
+      <c r="G80" s="96"/>
     </row>
     <row r="81" spans="1:7" s="51" customFormat="1">
       <c r="A81" s="56" t="s">
@@ -7072,23 +7072,23 @@
       <c r="A85" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B85" s="94"/>
-      <c r="C85" s="95"/>
-      <c r="D85" s="95"/>
-      <c r="E85" s="95"/>
-      <c r="F85" s="95"/>
-      <c r="G85" s="96"/>
+      <c r="B85" s="88"/>
+      <c r="C85" s="89"/>
+      <c r="D85" s="89"/>
+      <c r="E85" s="89"/>
+      <c r="F85" s="89"/>
+      <c r="G85" s="90"/>
     </row>
     <row r="86" spans="1:7" s="51" customFormat="1">
       <c r="A86" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="B86" s="88" t="s">
+      <c r="B86" s="91" t="s">
         <v>136</v>
       </c>
-      <c r="C86" s="89"/>
-      <c r="D86" s="89"/>
-      <c r="E86" s="90"/>
+      <c r="C86" s="92"/>
+      <c r="D86" s="92"/>
+      <c r="E86" s="93"/>
       <c r="F86" s="53" t="s">
         <v>87</v>
       </c>
@@ -7101,14 +7101,14 @@
       <c r="A87" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B87" s="91" t="s">
+      <c r="B87" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C87" s="92"/>
-      <c r="D87" s="92"/>
-      <c r="E87" s="92"/>
-      <c r="F87" s="92"/>
-      <c r="G87" s="93"/>
+      <c r="C87" s="95"/>
+      <c r="D87" s="95"/>
+      <c r="E87" s="95"/>
+      <c r="F87" s="95"/>
+      <c r="G87" s="96"/>
     </row>
     <row r="88" spans="1:7" s="51" customFormat="1">
       <c r="A88" s="56" t="s">
@@ -7207,23 +7207,23 @@
       <c r="A93" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B93" s="94"/>
-      <c r="C93" s="95"/>
-      <c r="D93" s="95"/>
-      <c r="E93" s="95"/>
-      <c r="F93" s="95"/>
-      <c r="G93" s="96"/>
+      <c r="B93" s="88"/>
+      <c r="C93" s="89"/>
+      <c r="D93" s="89"/>
+      <c r="E93" s="89"/>
+      <c r="F93" s="89"/>
+      <c r="G93" s="90"/>
     </row>
     <row r="94" spans="1:7" s="51" customFormat="1">
       <c r="A94" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="B94" s="88" t="s">
+      <c r="B94" s="91" t="s">
         <v>140</v>
       </c>
-      <c r="C94" s="89"/>
-      <c r="D94" s="89"/>
-      <c r="E94" s="90"/>
+      <c r="C94" s="92"/>
+      <c r="D94" s="92"/>
+      <c r="E94" s="93"/>
       <c r="F94" s="53" t="s">
         <v>87</v>
       </c>
@@ -7236,14 +7236,14 @@
       <c r="A95" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B95" s="91" t="s">
+      <c r="B95" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C95" s="92"/>
-      <c r="D95" s="92"/>
-      <c r="E95" s="92"/>
-      <c r="F95" s="92"/>
-      <c r="G95" s="93"/>
+      <c r="C95" s="95"/>
+      <c r="D95" s="95"/>
+      <c r="E95" s="95"/>
+      <c r="F95" s="95"/>
+      <c r="G95" s="96"/>
     </row>
     <row r="96" spans="1:7" s="51" customFormat="1">
       <c r="A96" s="56" t="s">
@@ -7340,23 +7340,23 @@
       <c r="A101" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B101" s="94"/>
-      <c r="C101" s="95"/>
-      <c r="D101" s="95"/>
-      <c r="E101" s="95"/>
-      <c r="F101" s="95"/>
-      <c r="G101" s="96"/>
+      <c r="B101" s="88"/>
+      <c r="C101" s="89"/>
+      <c r="D101" s="89"/>
+      <c r="E101" s="89"/>
+      <c r="F101" s="89"/>
+      <c r="G101" s="90"/>
     </row>
     <row r="102" spans="1:7" s="51" customFormat="1">
       <c r="A102" s="52" t="s">
         <v>139</v>
       </c>
-      <c r="B102" s="88" t="s">
+      <c r="B102" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="C102" s="89"/>
-      <c r="D102" s="89"/>
-      <c r="E102" s="90"/>
+      <c r="C102" s="92"/>
+      <c r="D102" s="92"/>
+      <c r="E102" s="93"/>
       <c r="F102" s="53" t="s">
         <v>87</v>
       </c>
@@ -7369,14 +7369,14 @@
       <c r="A103" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B103" s="91" t="s">
+      <c r="B103" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C103" s="92"/>
-      <c r="D103" s="92"/>
-      <c r="E103" s="92"/>
-      <c r="F103" s="92"/>
-      <c r="G103" s="93"/>
+      <c r="C103" s="95"/>
+      <c r="D103" s="95"/>
+      <c r="E103" s="95"/>
+      <c r="F103" s="95"/>
+      <c r="G103" s="96"/>
     </row>
     <row r="104" spans="1:7" s="51" customFormat="1">
       <c r="A104" s="56" t="s">
@@ -7490,23 +7490,23 @@
       <c r="A110" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B110" s="94"/>
-      <c r="C110" s="95"/>
-      <c r="D110" s="95"/>
-      <c r="E110" s="95"/>
-      <c r="F110" s="95"/>
-      <c r="G110" s="96"/>
+      <c r="B110" s="88"/>
+      <c r="C110" s="89"/>
+      <c r="D110" s="89"/>
+      <c r="E110" s="89"/>
+      <c r="F110" s="89"/>
+      <c r="G110" s="90"/>
     </row>
     <row r="111" spans="1:7" s="51" customFormat="1">
       <c r="A111" s="52" t="s">
         <v>142</v>
       </c>
-      <c r="B111" s="88" t="s">
+      <c r="B111" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="C111" s="89"/>
-      <c r="D111" s="89"/>
-      <c r="E111" s="90"/>
+      <c r="C111" s="92"/>
+      <c r="D111" s="92"/>
+      <c r="E111" s="93"/>
       <c r="F111" s="53" t="s">
         <v>87</v>
       </c>
@@ -7519,14 +7519,14 @@
       <c r="A112" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B112" s="91" t="s">
+      <c r="B112" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C112" s="92"/>
-      <c r="D112" s="92"/>
-      <c r="E112" s="92"/>
-      <c r="F112" s="92"/>
-      <c r="G112" s="93"/>
+      <c r="C112" s="95"/>
+      <c r="D112" s="95"/>
+      <c r="E112" s="95"/>
+      <c r="F112" s="95"/>
+      <c r="G112" s="96"/>
     </row>
     <row r="113" spans="1:7" s="51" customFormat="1">
       <c r="A113" s="56" t="s">
@@ -7608,23 +7608,23 @@
       <c r="A117" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B117" s="94"/>
-      <c r="C117" s="95"/>
-      <c r="D117" s="95"/>
-      <c r="E117" s="95"/>
-      <c r="F117" s="95"/>
-      <c r="G117" s="96"/>
+      <c r="B117" s="88"/>
+      <c r="C117" s="89"/>
+      <c r="D117" s="89"/>
+      <c r="E117" s="89"/>
+      <c r="F117" s="89"/>
+      <c r="G117" s="90"/>
     </row>
     <row r="118" spans="1:7" s="51" customFormat="1">
       <c r="A118" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="B118" s="88" t="s">
+      <c r="B118" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="C118" s="89"/>
-      <c r="D118" s="89"/>
-      <c r="E118" s="90"/>
+      <c r="C118" s="92"/>
+      <c r="D118" s="92"/>
+      <c r="E118" s="93"/>
       <c r="F118" s="53" t="s">
         <v>87</v>
       </c>
@@ -7637,14 +7637,14 @@
       <c r="A119" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B119" s="91" t="s">
+      <c r="B119" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C119" s="92"/>
-      <c r="D119" s="92"/>
-      <c r="E119" s="92"/>
-      <c r="F119" s="92"/>
-      <c r="G119" s="93"/>
+      <c r="C119" s="95"/>
+      <c r="D119" s="95"/>
+      <c r="E119" s="95"/>
+      <c r="F119" s="95"/>
+      <c r="G119" s="96"/>
     </row>
     <row r="120" spans="1:7" s="51" customFormat="1">
       <c r="A120" s="56" t="s">
@@ -7724,23 +7724,23 @@
       <c r="A124" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B124" s="94"/>
-      <c r="C124" s="95"/>
-      <c r="D124" s="95"/>
-      <c r="E124" s="95"/>
-      <c r="F124" s="95"/>
-      <c r="G124" s="96"/>
+      <c r="B124" s="88"/>
+      <c r="C124" s="89"/>
+      <c r="D124" s="89"/>
+      <c r="E124" s="89"/>
+      <c r="F124" s="89"/>
+      <c r="G124" s="90"/>
     </row>
     <row r="125" spans="1:7" s="51" customFormat="1">
       <c r="A125" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="B125" s="88" t="s">
+      <c r="B125" s="91" t="s">
         <v>157</v>
       </c>
-      <c r="C125" s="89"/>
-      <c r="D125" s="89"/>
-      <c r="E125" s="90"/>
+      <c r="C125" s="92"/>
+      <c r="D125" s="92"/>
+      <c r="E125" s="93"/>
       <c r="F125" s="53" t="s">
         <v>87</v>
       </c>
@@ -7753,14 +7753,14 @@
       <c r="A126" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B126" s="91" t="s">
+      <c r="B126" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C126" s="92"/>
-      <c r="D126" s="92"/>
-      <c r="E126" s="92"/>
-      <c r="F126" s="92"/>
-      <c r="G126" s="93"/>
+      <c r="C126" s="95"/>
+      <c r="D126" s="95"/>
+      <c r="E126" s="95"/>
+      <c r="F126" s="95"/>
+      <c r="G126" s="96"/>
     </row>
     <row r="127" spans="1:7" s="51" customFormat="1">
       <c r="A127" s="56" t="s">
@@ -7857,23 +7857,23 @@
       <c r="A132" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B132" s="94"/>
-      <c r="C132" s="95"/>
-      <c r="D132" s="95"/>
-      <c r="E132" s="95"/>
-      <c r="F132" s="95"/>
-      <c r="G132" s="96"/>
+      <c r="B132" s="88"/>
+      <c r="C132" s="89"/>
+      <c r="D132" s="89"/>
+      <c r="E132" s="89"/>
+      <c r="F132" s="89"/>
+      <c r="G132" s="90"/>
     </row>
     <row r="133" spans="1:7" s="51" customFormat="1">
       <c r="A133" s="52" t="s">
         <v>156</v>
       </c>
-      <c r="B133" s="88" t="s">
+      <c r="B133" s="91" t="s">
         <v>163</v>
       </c>
-      <c r="C133" s="89"/>
-      <c r="D133" s="89"/>
-      <c r="E133" s="90"/>
+      <c r="C133" s="92"/>
+      <c r="D133" s="92"/>
+      <c r="E133" s="93"/>
       <c r="F133" s="53" t="s">
         <v>87</v>
       </c>
@@ -7886,14 +7886,14 @@
       <c r="A134" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B134" s="91" t="s">
+      <c r="B134" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C134" s="92"/>
-      <c r="D134" s="92"/>
-      <c r="E134" s="92"/>
-      <c r="F134" s="92"/>
-      <c r="G134" s="93"/>
+      <c r="C134" s="95"/>
+      <c r="D134" s="95"/>
+      <c r="E134" s="95"/>
+      <c r="F134" s="95"/>
+      <c r="G134" s="96"/>
     </row>
     <row r="135" spans="1:7" s="51" customFormat="1">
       <c r="A135" s="56" t="s">
@@ -7973,23 +7973,23 @@
       <c r="A139" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B139" s="94"/>
-      <c r="C139" s="95"/>
-      <c r="D139" s="95"/>
-      <c r="E139" s="95"/>
-      <c r="F139" s="95"/>
-      <c r="G139" s="96"/>
+      <c r="B139" s="88"/>
+      <c r="C139" s="89"/>
+      <c r="D139" s="89"/>
+      <c r="E139" s="89"/>
+      <c r="F139" s="89"/>
+      <c r="G139" s="90"/>
     </row>
     <row r="140" spans="1:7" s="51" customFormat="1">
       <c r="A140" s="52" t="s">
         <v>161</v>
       </c>
-      <c r="B140" s="88" t="s">
+      <c r="B140" s="91" t="s">
         <v>164</v>
       </c>
-      <c r="C140" s="89"/>
-      <c r="D140" s="89"/>
-      <c r="E140" s="90"/>
+      <c r="C140" s="92"/>
+      <c r="D140" s="92"/>
+      <c r="E140" s="93"/>
       <c r="F140" s="53" t="s">
         <v>87</v>
       </c>
@@ -8002,14 +8002,14 @@
       <c r="A141" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B141" s="91" t="s">
+      <c r="B141" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C141" s="92"/>
-      <c r="D141" s="92"/>
-      <c r="E141" s="92"/>
-      <c r="F141" s="92"/>
-      <c r="G141" s="93"/>
+      <c r="C141" s="95"/>
+      <c r="D141" s="95"/>
+      <c r="E141" s="95"/>
+      <c r="F141" s="95"/>
+      <c r="G141" s="96"/>
     </row>
     <row r="142" spans="1:7" s="51" customFormat="1">
       <c r="A142" s="56" t="s">
@@ -8089,23 +8089,23 @@
       <c r="A146" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B146" s="94"/>
-      <c r="C146" s="95"/>
-      <c r="D146" s="95"/>
-      <c r="E146" s="95"/>
-      <c r="F146" s="95"/>
-      <c r="G146" s="96"/>
+      <c r="B146" s="88"/>
+      <c r="C146" s="89"/>
+      <c r="D146" s="89"/>
+      <c r="E146" s="89"/>
+      <c r="F146" s="89"/>
+      <c r="G146" s="90"/>
     </row>
     <row r="147" spans="1:7" s="51" customFormat="1">
       <c r="A147" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="B147" s="88" t="s">
+      <c r="B147" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="C147" s="89"/>
-      <c r="D147" s="89"/>
-      <c r="E147" s="90"/>
+      <c r="C147" s="92"/>
+      <c r="D147" s="92"/>
+      <c r="E147" s="93"/>
       <c r="F147" s="53" t="s">
         <v>87</v>
       </c>
@@ -8118,14 +8118,14 @@
       <c r="A148" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B148" s="91" t="s">
+      <c r="B148" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C148" s="92"/>
-      <c r="D148" s="92"/>
-      <c r="E148" s="92"/>
-      <c r="F148" s="92"/>
-      <c r="G148" s="93"/>
+      <c r="C148" s="95"/>
+      <c r="D148" s="95"/>
+      <c r="E148" s="95"/>
+      <c r="F148" s="95"/>
+      <c r="G148" s="96"/>
     </row>
     <row r="149" spans="1:7" s="51" customFormat="1">
       <c r="A149" s="56" t="s">
@@ -8205,23 +8205,23 @@
       <c r="A153" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B153" s="94"/>
-      <c r="C153" s="95"/>
-      <c r="D153" s="95"/>
-      <c r="E153" s="95"/>
-      <c r="F153" s="95"/>
-      <c r="G153" s="96"/>
+      <c r="B153" s="88"/>
+      <c r="C153" s="89"/>
+      <c r="D153" s="89"/>
+      <c r="E153" s="89"/>
+      <c r="F153" s="89"/>
+      <c r="G153" s="90"/>
     </row>
     <row r="154" spans="1:7" s="51" customFormat="1">
       <c r="A154" s="52" t="s">
         <v>170</v>
       </c>
-      <c r="B154" s="88" t="s">
+      <c r="B154" s="91" t="s">
         <v>171</v>
       </c>
-      <c r="C154" s="89"/>
-      <c r="D154" s="89"/>
-      <c r="E154" s="90"/>
+      <c r="C154" s="92"/>
+      <c r="D154" s="92"/>
+      <c r="E154" s="93"/>
       <c r="F154" s="53" t="s">
         <v>87</v>
       </c>
@@ -8234,14 +8234,14 @@
       <c r="A155" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B155" s="91" t="s">
+      <c r="B155" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C155" s="92"/>
-      <c r="D155" s="92"/>
-      <c r="E155" s="92"/>
-      <c r="F155" s="92"/>
-      <c r="G155" s="93"/>
+      <c r="C155" s="95"/>
+      <c r="D155" s="95"/>
+      <c r="E155" s="95"/>
+      <c r="F155" s="95"/>
+      <c r="G155" s="96"/>
     </row>
     <row r="156" spans="1:7" s="51" customFormat="1">
       <c r="A156" s="56" t="s">
@@ -8304,23 +8304,23 @@
       <c r="A159" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B159" s="94"/>
-      <c r="C159" s="95"/>
-      <c r="D159" s="95"/>
-      <c r="E159" s="95"/>
-      <c r="F159" s="95"/>
-      <c r="G159" s="96"/>
+      <c r="B159" s="88"/>
+      <c r="C159" s="89"/>
+      <c r="D159" s="89"/>
+      <c r="E159" s="89"/>
+      <c r="F159" s="89"/>
+      <c r="G159" s="90"/>
     </row>
     <row r="160" spans="1:7" s="51" customFormat="1">
       <c r="A160" s="52" t="s">
         <v>175</v>
       </c>
-      <c r="B160" s="88" t="s">
+      <c r="B160" s="91" t="s">
         <v>173</v>
       </c>
-      <c r="C160" s="89"/>
-      <c r="D160" s="89"/>
-      <c r="E160" s="90"/>
+      <c r="C160" s="92"/>
+      <c r="D160" s="92"/>
+      <c r="E160" s="93"/>
       <c r="F160" s="53" t="s">
         <v>87</v>
       </c>
@@ -8333,14 +8333,14 @@
       <c r="A161" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B161" s="91" t="s">
+      <c r="B161" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C161" s="92"/>
-      <c r="D161" s="92"/>
-      <c r="E161" s="92"/>
-      <c r="F161" s="92"/>
-      <c r="G161" s="93"/>
+      <c r="C161" s="95"/>
+      <c r="D161" s="95"/>
+      <c r="E161" s="95"/>
+      <c r="F161" s="95"/>
+      <c r="G161" s="96"/>
     </row>
     <row r="162" spans="1:7" s="51" customFormat="1">
       <c r="A162" s="56" t="s">
@@ -8420,23 +8420,23 @@
       <c r="A166" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B166" s="94"/>
-      <c r="C166" s="95"/>
-      <c r="D166" s="95"/>
-      <c r="E166" s="95"/>
-      <c r="F166" s="95"/>
-      <c r="G166" s="96"/>
+      <c r="B166" s="88"/>
+      <c r="C166" s="89"/>
+      <c r="D166" s="89"/>
+      <c r="E166" s="89"/>
+      <c r="F166" s="89"/>
+      <c r="G166" s="90"/>
     </row>
     <row r="167" spans="1:7" s="51" customFormat="1">
       <c r="A167" s="52" t="s">
         <v>179</v>
       </c>
-      <c r="B167" s="88" t="s">
+      <c r="B167" s="91" t="s">
         <v>178</v>
       </c>
-      <c r="C167" s="89"/>
-      <c r="D167" s="89"/>
-      <c r="E167" s="90"/>
+      <c r="C167" s="92"/>
+      <c r="D167" s="92"/>
+      <c r="E167" s="93"/>
       <c r="F167" s="53" t="s">
         <v>87</v>
       </c>
@@ -8449,14 +8449,14 @@
       <c r="A168" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B168" s="91" t="s">
+      <c r="B168" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C168" s="92"/>
-      <c r="D168" s="92"/>
-      <c r="E168" s="92"/>
-      <c r="F168" s="92"/>
-      <c r="G168" s="93"/>
+      <c r="C168" s="95"/>
+      <c r="D168" s="95"/>
+      <c r="E168" s="95"/>
+      <c r="F168" s="95"/>
+      <c r="G168" s="96"/>
     </row>
     <row r="169" spans="1:7" s="51" customFormat="1">
       <c r="A169" s="56" t="s">
@@ -8536,23 +8536,23 @@
       <c r="A173" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B173" s="94"/>
-      <c r="C173" s="95"/>
-      <c r="D173" s="95"/>
-      <c r="E173" s="95"/>
-      <c r="F173" s="95"/>
-      <c r="G173" s="96"/>
+      <c r="B173" s="88"/>
+      <c r="C173" s="89"/>
+      <c r="D173" s="89"/>
+      <c r="E173" s="89"/>
+      <c r="F173" s="89"/>
+      <c r="G173" s="90"/>
     </row>
     <row r="174" spans="1:7" s="51" customFormat="1">
       <c r="A174" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="B174" s="88" t="s">
+      <c r="B174" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="C174" s="89"/>
-      <c r="D174" s="89"/>
-      <c r="E174" s="90"/>
+      <c r="C174" s="92"/>
+      <c r="D174" s="92"/>
+      <c r="E174" s="93"/>
       <c r="F174" s="53" t="s">
         <v>87</v>
       </c>
@@ -8565,14 +8565,14 @@
       <c r="A175" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B175" s="91" t="s">
+      <c r="B175" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C175" s="92"/>
-      <c r="D175" s="92"/>
-      <c r="E175" s="92"/>
-      <c r="F175" s="92"/>
-      <c r="G175" s="93"/>
+      <c r="C175" s="95"/>
+      <c r="D175" s="95"/>
+      <c r="E175" s="95"/>
+      <c r="F175" s="95"/>
+      <c r="G175" s="96"/>
     </row>
     <row r="176" spans="1:7" s="51" customFormat="1">
       <c r="A176" s="56" t="s">
@@ -8675,23 +8675,23 @@
       <c r="A181" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B181" s="94"/>
-      <c r="C181" s="95"/>
-      <c r="D181" s="95"/>
-      <c r="E181" s="95"/>
-      <c r="F181" s="95"/>
-      <c r="G181" s="96"/>
+      <c r="B181" s="88"/>
+      <c r="C181" s="89"/>
+      <c r="D181" s="89"/>
+      <c r="E181" s="89"/>
+      <c r="F181" s="89"/>
+      <c r="G181" s="90"/>
     </row>
     <row r="182" spans="1:7" s="51" customFormat="1">
       <c r="A182" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="B182" s="88" t="s">
+      <c r="B182" s="91" t="s">
         <v>194</v>
       </c>
-      <c r="C182" s="89"/>
-      <c r="D182" s="89"/>
-      <c r="E182" s="90"/>
+      <c r="C182" s="92"/>
+      <c r="D182" s="92"/>
+      <c r="E182" s="93"/>
       <c r="F182" s="53" t="s">
         <v>87</v>
       </c>
@@ -8704,14 +8704,14 @@
       <c r="A183" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B183" s="91" t="s">
+      <c r="B183" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C183" s="92"/>
-      <c r="D183" s="92"/>
-      <c r="E183" s="92"/>
-      <c r="F183" s="92"/>
-      <c r="G183" s="93"/>
+      <c r="C183" s="95"/>
+      <c r="D183" s="95"/>
+      <c r="E183" s="95"/>
+      <c r="F183" s="95"/>
+      <c r="G183" s="96"/>
     </row>
     <row r="184" spans="1:7" s="51" customFormat="1">
       <c r="A184" s="56" t="s">
@@ -8791,23 +8791,23 @@
       <c r="A188" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B188" s="94"/>
-      <c r="C188" s="95"/>
-      <c r="D188" s="95"/>
-      <c r="E188" s="95"/>
-      <c r="F188" s="95"/>
-      <c r="G188" s="96"/>
+      <c r="B188" s="88"/>
+      <c r="C188" s="89"/>
+      <c r="D188" s="89"/>
+      <c r="E188" s="89"/>
+      <c r="F188" s="89"/>
+      <c r="G188" s="90"/>
     </row>
     <row r="189" spans="1:7" s="51" customFormat="1">
       <c r="A189" s="52" t="s">
         <v>196</v>
       </c>
-      <c r="B189" s="88" t="s">
+      <c r="B189" s="91" t="s">
         <v>197</v>
       </c>
-      <c r="C189" s="89"/>
-      <c r="D189" s="89"/>
-      <c r="E189" s="90"/>
+      <c r="C189" s="92"/>
+      <c r="D189" s="92"/>
+      <c r="E189" s="93"/>
       <c r="F189" s="53" t="s">
         <v>87</v>
       </c>
@@ -8820,14 +8820,14 @@
       <c r="A190" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B190" s="91" t="s">
+      <c r="B190" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C190" s="92"/>
-      <c r="D190" s="92"/>
-      <c r="E190" s="92"/>
-      <c r="F190" s="92"/>
-      <c r="G190" s="93"/>
+      <c r="C190" s="95"/>
+      <c r="D190" s="95"/>
+      <c r="E190" s="95"/>
+      <c r="F190" s="95"/>
+      <c r="G190" s="96"/>
     </row>
     <row r="191" spans="1:7" s="51" customFormat="1">
       <c r="A191" s="56" t="s">
@@ -8909,23 +8909,23 @@
       <c r="A195" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B195" s="94"/>
-      <c r="C195" s="95"/>
-      <c r="D195" s="95"/>
-      <c r="E195" s="95"/>
-      <c r="F195" s="95"/>
-      <c r="G195" s="96"/>
+      <c r="B195" s="88"/>
+      <c r="C195" s="89"/>
+      <c r="D195" s="89"/>
+      <c r="E195" s="89"/>
+      <c r="F195" s="89"/>
+      <c r="G195" s="90"/>
     </row>
     <row r="196" spans="1:7">
       <c r="A196" s="52" t="s">
         <v>227</v>
       </c>
-      <c r="B196" s="88" t="s">
+      <c r="B196" s="91" t="s">
         <v>224</v>
       </c>
-      <c r="C196" s="89"/>
-      <c r="D196" s="89"/>
-      <c r="E196" s="90"/>
+      <c r="C196" s="92"/>
+      <c r="D196" s="92"/>
+      <c r="E196" s="93"/>
       <c r="F196" s="53" t="s">
         <v>87</v>
       </c>
@@ -8938,14 +8938,14 @@
       <c r="A197" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B197" s="91" t="s">
+      <c r="B197" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="C197" s="92"/>
-      <c r="D197" s="92"/>
-      <c r="E197" s="92"/>
-      <c r="F197" s="92"/>
-      <c r="G197" s="93"/>
+      <c r="C197" s="95"/>
+      <c r="D197" s="95"/>
+      <c r="E197" s="95"/>
+      <c r="F197" s="95"/>
+      <c r="G197" s="96"/>
     </row>
     <row r="198" spans="1:7">
       <c r="A198" s="56" t="s">
@@ -9078,12 +9078,12 @@
       <c r="A205" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="B205" s="94"/>
-      <c r="C205" s="95"/>
-      <c r="D205" s="95"/>
-      <c r="E205" s="95"/>
-      <c r="F205" s="95"/>
-      <c r="G205" s="96"/>
+      <c r="B205" s="88"/>
+      <c r="C205" s="89"/>
+      <c r="D205" s="89"/>
+      <c r="E205" s="89"/>
+      <c r="F205" s="89"/>
+      <c r="G205" s="90"/>
     </row>
     <row r="206" spans="1:7">
       <c r="A206" s="32"/>
@@ -15771,69 +15771,6 @@
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="B188:G188"/>
-    <mergeCell ref="B189:E189"/>
-    <mergeCell ref="B190:G190"/>
-    <mergeCell ref="B195:G195"/>
-    <mergeCell ref="B174:E174"/>
-    <mergeCell ref="B175:G175"/>
-    <mergeCell ref="B181:G181"/>
-    <mergeCell ref="B182:E182"/>
-    <mergeCell ref="B183:G183"/>
-    <mergeCell ref="B154:E154"/>
-    <mergeCell ref="B155:G155"/>
-    <mergeCell ref="B159:G159"/>
-    <mergeCell ref="B160:E160"/>
-    <mergeCell ref="B173:G173"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="B66:G66"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B71:G71"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="B73:G73"/>
-    <mergeCell ref="B78:G78"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="B80:G80"/>
-    <mergeCell ref="B85:G85"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B87:G87"/>
-    <mergeCell ref="B93:G93"/>
-    <mergeCell ref="B94:E94"/>
-    <mergeCell ref="B95:G95"/>
-    <mergeCell ref="B101:G101"/>
-    <mergeCell ref="B102:E102"/>
-    <mergeCell ref="B103:G103"/>
-    <mergeCell ref="B110:G110"/>
-    <mergeCell ref="B111:E111"/>
-    <mergeCell ref="B112:G112"/>
-    <mergeCell ref="B117:G117"/>
-    <mergeCell ref="B118:E118"/>
-    <mergeCell ref="B119:G119"/>
-    <mergeCell ref="B124:G124"/>
-    <mergeCell ref="B125:E125"/>
-    <mergeCell ref="B126:G126"/>
-    <mergeCell ref="B132:G132"/>
     <mergeCell ref="B196:E196"/>
     <mergeCell ref="B197:G197"/>
     <mergeCell ref="B205:G205"/>
@@ -15850,6 +15787,69 @@
     <mergeCell ref="B167:E167"/>
     <mergeCell ref="B168:G168"/>
     <mergeCell ref="B153:G153"/>
+    <mergeCell ref="B119:G119"/>
+    <mergeCell ref="B124:G124"/>
+    <mergeCell ref="B125:E125"/>
+    <mergeCell ref="B126:G126"/>
+    <mergeCell ref="B132:G132"/>
+    <mergeCell ref="B110:G110"/>
+    <mergeCell ref="B111:E111"/>
+    <mergeCell ref="B112:G112"/>
+    <mergeCell ref="B117:G117"/>
+    <mergeCell ref="B118:E118"/>
+    <mergeCell ref="B94:E94"/>
+    <mergeCell ref="B95:G95"/>
+    <mergeCell ref="B101:G101"/>
+    <mergeCell ref="B102:E102"/>
+    <mergeCell ref="B103:G103"/>
+    <mergeCell ref="B80:G80"/>
+    <mergeCell ref="B85:G85"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B87:G87"/>
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="B71:G71"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="B73:G73"/>
+    <mergeCell ref="B78:G78"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="B66:G66"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B41:G41"/>
+    <mergeCell ref="B154:E154"/>
+    <mergeCell ref="B155:G155"/>
+    <mergeCell ref="B159:G159"/>
+    <mergeCell ref="B160:E160"/>
+    <mergeCell ref="B173:G173"/>
+    <mergeCell ref="B188:G188"/>
+    <mergeCell ref="B189:E189"/>
+    <mergeCell ref="B190:G190"/>
+    <mergeCell ref="B195:G195"/>
+    <mergeCell ref="B174:E174"/>
+    <mergeCell ref="B175:G175"/>
+    <mergeCell ref="B181:G181"/>
+    <mergeCell ref="B182:E182"/>
+    <mergeCell ref="B183:G183"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" showErrorMessage="1" promptTitle="Valid values include:" prompt="_x000a_" sqref="F431:F433 F438:F444 F657:F659 F647:F652 F449:F458 F463:F466 F471:F476 F481:F489 F494:F503 F508:F518 F523:F533 F549:F555 F577:F579 F538:F544 F560:F566 F571:F572 F584:F590 F595:F601 F617:F619 F606:F612 F624:F627 F632:F634 F639:F642 F21 F192:F194 F26:F29 F45:F47 F52:F55 F68:F70 F75:F77 F82:F84 F89:F92 F97:F100 F105:F109 F114:F116 F121:F123 F128:F131 F60:F63 F136:F138 F143:F145 F150:F152 F157:F158 F163:F165 F170:F172 F177:F180 F185:F187 F34:F40 F199:F204" xr:uid="{00000000-0002-0000-0200-000000000000}">

</xml_diff>